<commit_message>
new excel file added for developing purpose
</commit_message>
<xml_diff>
--- a/seo_paper_02_severn.xlsx
+++ b/seo_paper_02_severn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335"/>
+    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setting" sheetId="8" r:id="rId1"/>
@@ -17,6 +17,9 @@
     <sheet name="ماکیناو" sheetId="15" state="hidden" r:id="rId8"/>
     <sheet name="سورن سفارش نوری" sheetId="13" state="hidden" r:id="rId9"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId10"/>
+  </externalReferences>
   <definedNames>
     <definedName name="Delta_T__seconds">Setting!$B$10</definedName>
     <definedName name="Delta_X">Setting!$H$10:$H$17</definedName>
@@ -104,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="114">
   <si>
     <t>Project Name</t>
   </si>
@@ -440,6 +443,12 @@
   </si>
   <si>
     <t>St7 @ 13.775 (km)</t>
+  </si>
+  <si>
+    <t>X cells for evaluation and comparison with obsered</t>
+  </si>
+  <si>
+    <t>Observed Concentration [ppm] using formula2</t>
   </si>
 </sst>
 </file>
@@ -738,7 +747,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -952,6 +961,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor theme="6" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -1391,7 +1406,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1643,6 +1658,36 @@
     <xf numFmtId="164" fontId="20" fillId="32" borderId="7" xfId="37" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="39" borderId="14" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="14" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="39" borderId="14" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="14" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="39" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="39" borderId="21" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1650,6 +1695,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="7" xfId="37" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="7" xfId="37" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1699,7 +1750,56 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="45">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Cutive Mono"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Cutive Mono"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4198,86 +4298,121 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Setting"/>
+      <sheetName val="Reach Propertise"/>
+      <sheetName val="Initial Concentration"/>
+      <sheetName val="Loading"/>
+      <sheetName val="hidden tab"/>
+      <sheetName val="LDC"/>
+      <sheetName val="چاتا"/>
+      <sheetName val="ماکیناو"/>
+      <sheetName val="سورن سفارش نوری"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AN8" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41" tableBorderDxfId="40" headerRowCellStyle="Note" dataCellStyle="Note">
-  <autoFilter ref="A1:AN8"/>
-  <tableColumns count="40">
-    <tableColumn id="1" name="Name" dataDxfId="39"/>
-    <tableColumn id="2" name="Start point distance [meters]" dataDxfId="38"/>
-    <tableColumn id="3" name="End Point distance  [meters]" dataDxfId="37" dataCellStyle="Note"/>
-    <tableColumn id="4" name="Q [m3/sec]" dataDxfId="36"/>
-    <tableColumn id="5" name="Ti" dataDxfId="35" dataCellStyle="Note"/>
-    <tableColumn id="6" name="Tp" dataDxfId="34"/>
-    <tableColumn id="7" name="Tt" dataDxfId="33" dataCellStyle="Note"/>
-    <tableColumn id="8" name="Q average" dataDxfId="32" dataCellStyle="Note"/>
-    <tableColumn id="9" name="Drainage Area [km2]" dataDxfId="31" dataCellStyle="Note"/>
-    <tableColumn id="10" name="longitudinal slope" dataDxfId="30"/>
-    <tableColumn id="11" name="depth [meters]" dataDxfId="29"/>
-    <tableColumn id="12" name="width [meters]" dataDxfId="28"/>
-    <tableColumn id="13" name="Cup" dataDxfId="27"/>
-    <tableColumn id="14" name="Inj Mass" dataDxfId="26" dataCellStyle="Note"/>
-    <tableColumn id="15" name="R ratio" dataDxfId="25" dataCellStyle="Note"/>
-    <tableColumn id="16" name="Ref" dataDxfId="24" dataCellStyle="Note"/>
-    <tableColumn id="17" name="Calculated Velocity [meters/sec]" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AP8" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" tableBorderDxfId="42" headerRowCellStyle="Note" dataCellStyle="Note">
+  <autoFilter ref="A1:AP8"/>
+  <tableColumns count="42">
+    <tableColumn id="1" name="Name" dataDxfId="41"/>
+    <tableColumn id="2" name="Start point distance [meters]" dataDxfId="40"/>
+    <tableColumn id="3" name="End Point distance  [meters]" dataDxfId="39" dataCellStyle="Note"/>
+    <tableColumn id="4" name="Q [m3/sec]" dataDxfId="38"/>
+    <tableColumn id="5" name="Ti" dataDxfId="37" dataCellStyle="Note"/>
+    <tableColumn id="6" name="Tp" dataDxfId="36"/>
+    <tableColumn id="7" name="Tt" dataDxfId="35" dataCellStyle="Note"/>
+    <tableColumn id="8" name="Q average" dataDxfId="34" dataCellStyle="Note"/>
+    <tableColumn id="9" name="Drainage Area [km2]" dataDxfId="33" dataCellStyle="Note"/>
+    <tableColumn id="10" name="longitudinal slope" dataDxfId="32"/>
+    <tableColumn id="11" name="depth [meters]" dataDxfId="31"/>
+    <tableColumn id="12" name="width [meters]" dataDxfId="30"/>
+    <tableColumn id="13" name="Cup" dataDxfId="29"/>
+    <tableColumn id="14" name="Inj Mass" dataDxfId="28" dataCellStyle="Note"/>
+    <tableColumn id="15" name="R ratio" dataDxfId="27" dataCellStyle="Note"/>
+    <tableColumn id="16" name="Ref" dataDxfId="26" dataCellStyle="Note"/>
+    <tableColumn id="17" name="Calculated Velocity [meters/sec]" dataDxfId="25">
       <calculatedColumnFormula>Table1[Q '[m3/sec']]/(Table1[depth '[meters']]*Table1[width '[meters']])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="calculated time [hours]" dataDxfId="22" dataCellStyle="Note">
+    <tableColumn id="18" name="calculated time [hours]" dataDxfId="24" dataCellStyle="Note">
       <calculatedColumnFormula>(Table1[[#This Row],[Reach Length '[meters']]]/(Table1[[#This Row],[Q '[m3/sec']]]/(Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]])))/3600</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Observed Velocity [meters / seconds]" dataDxfId="21" dataCellStyle="Note">
+    <tableColumn id="19" name="Observed Velocity [meters / seconds]" dataDxfId="23" dataCellStyle="Note">
       <calculatedColumnFormula>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="ɳ" dataDxfId="20"/>
-    <tableColumn id="21" name="river side slope" dataDxfId="19"/>
-    <tableColumn id="22" name="Initial Concentration [mgr/Lit]" dataDxfId="18"/>
-    <tableColumn id="23" name="End Point of Reach [km]" dataDxfId="17" dataCellStyle="Note">
+    <tableColumn id="20" name="ɳ" dataDxfId="22"/>
+    <tableColumn id="21" name="river side slope" dataDxfId="21"/>
+    <tableColumn id="22" name="Initial Concentration [mgr/Lit]" dataDxfId="20"/>
+    <tableColumn id="23" name="End Point of Reach [km]" dataDxfId="19" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[End Point distance  '[meters']]]/1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="Observed Concentration [ppm]" dataDxfId="16"/>
-    <tableColumn id="25" name="Error in Calc time Vs Obs Time" dataDxfId="15" dataCellStyle="Percent">
+    <tableColumn id="24" name="Observed Concentration [ppm]" dataDxfId="18"/>
+    <tableColumn id="25" name="Error in Calc time Vs Obs Time" dataDxfId="17" dataCellStyle="Percent">
       <calculatedColumnFormula>IF(AVERAGE(Table1[[#This Row],[Error Ti]]&lt;=AVERAGE(Table1[[#This Row],[Error Tp]])),"use Ti","use Tp")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="Reach Length [meters]" dataDxfId="14" dataCellStyle="Note">
+    <tableColumn id="26" name="Reach Length [meters]" dataDxfId="16" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[End Point distance  '[meters']]]-Table1[[#This Row],[Start point distance '[meters']]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" name="Reach Time (seconds)" dataDxfId="13" dataCellStyle="Note">
+    <tableColumn id="39" name="Reach Time (seconds)" dataDxfId="15" dataCellStyle="Note">
       <calculatedColumnFormula>(Table1[[#This Row],[Tp]]-AN2)*3600</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="Time Cell" dataDxfId="12" dataCellStyle="Note">
+    <tableColumn id="27" name="Time Cell" dataDxfId="14" dataCellStyle="Note">
       <calculatedColumnFormula>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" name="End Spatial Cell" dataDxfId="11" dataCellStyle="Note">
+    <tableColumn id="37" name="End Spatial Cell" dataDxfId="13" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" name="Start Spatial Cell" dataDxfId="10" dataCellStyle="Note">
+    <tableColumn id="38" name="Start Spatial Cell" dataDxfId="12" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" name="Delta T" dataDxfId="9" dataCellStyle="Note">
+    <tableColumn id="28" name="Delta T" dataDxfId="11" dataCellStyle="Note">
       <calculatedColumnFormula>Delta_T__seconds</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" name="Error Ti" dataDxfId="8" dataCellStyle="Percent">
+    <tableColumn id="29" name="Error Ti" dataDxfId="10" dataCellStyle="Percent">
       <calculatedColumnFormula>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" name="Error Tp" dataDxfId="7" dataCellStyle="Percent">
+    <tableColumn id="30" name="Error Tp" dataDxfId="9" dataCellStyle="Percent">
       <calculatedColumnFormula>(('Reach Propertise'!$F2-'Reach Propertise'!$R2)/'Reach Propertise'!$F2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" name="Error Tt" dataDxfId="6" dataCellStyle="Percent">
+    <tableColumn id="31" name="Error Tt" dataDxfId="8" dataCellStyle="Percent">
       <calculatedColumnFormula>((Table1[[#This Row],[Tt]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Tt]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" name="Column1" dataDxfId="5" dataCellStyle="Percent">
+    <tableColumn id="32" name="Column1" dataDxfId="7" dataCellStyle="Percent">
       <calculatedColumnFormula>Table1[[#This Row],[width '[meters']]]/Table1[[#This Row],[depth '[meters']]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" name="Vi" dataDxfId="4" dataCellStyle="Note">
+    <tableColumn id="33" name="Vi" dataDxfId="6" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" name="delta Tp" dataDxfId="3" dataCellStyle="Note">
+    <tableColumn id="34" name="delta Tp" dataDxfId="5" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="Column2" dataDxfId="2" dataCellStyle="Note"/>
-    <tableColumn id="36" name="Column3" dataDxfId="1" dataCellStyle="Note">
+    <tableColumn id="35" name="Column2" dataDxfId="4" dataCellStyle="Note"/>
+    <tableColumn id="36" name="Column3" dataDxfId="3" dataCellStyle="Note">
       <calculatedColumnFormula>'Reach Propertise'!$F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" name="Column4" dataDxfId="0" dataCellStyle="Note"/>
+    <tableColumn id="40" name="Column4" dataDxfId="2" dataCellStyle="Note"/>
+    <tableColumn id="41" name="X cells for evaluation and comparison with obsered" dataDxfId="0" dataCellStyle="Note">
+      <calculatedColumnFormula>FLOOR(C2:C8/Delta_X__meters,1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="42" name="Observed Concentration [ppm] using formula2" dataDxfId="1" dataCellStyle="Note">
+      <calculatedColumnFormula>((1/1000000)*[1]!Table1[[#This Row],[Cup]]*[1]!Table1[[#This Row],[R ratio]]*[1]!Table1[[#This Row],[Inj Mass]])/[1]!Table1[[#This Row],[Q '[m3/sec']]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4575,8 +4710,8 @@
   </sheetPr>
   <dimension ref="A1:X91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4824,7 +4959,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="53">
-        <v>1000</v>
+        <v>60</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -4854,7 +4989,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="53">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -4884,7 +5019,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="54" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -4914,12 +5049,13 @@
         <v>18</v>
       </c>
       <c r="B12" s="53">
-        <v>50</v>
+        <f>Delta_X__meters</f>
+        <v>60</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="8"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -4949,7 +5085,7 @@
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="8"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
@@ -4979,7 +5115,7 @@
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="8"/>
+      <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
@@ -5005,7 +5141,7 @@
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="8"/>
+      <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -5031,7 +5167,7 @@
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="8"/>
+      <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -5057,7 +5193,7 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="8"/>
+      <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
@@ -5083,7 +5219,7 @@
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="8"/>
+      <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
@@ -5109,7 +5245,7 @@
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="8"/>
+      <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
@@ -5135,7 +5271,7 @@
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="8"/>
+      <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
@@ -5161,7 +5297,7 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="8"/>
+      <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
@@ -6974,11 +7110,11 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:AN11"/>
+  <dimension ref="A1:AP21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="X2" sqref="X2:X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7016,10 +7152,13 @@
     <col min="36" max="36" width="9.140625" style="67"/>
     <col min="37" max="37" width="12.28515625" style="67" customWidth="1"/>
     <col min="38" max="39" width="11.140625" style="67" customWidth="1"/>
-    <col min="40" max="16384" width="9.140625" style="67"/>
+    <col min="40" max="40" width="9.140625" style="67"/>
+    <col min="41" max="41" width="34.5703125" style="67" customWidth="1"/>
+    <col min="42" max="42" width="23.5703125" style="67" customWidth="1"/>
+    <col min="43" max="16384" width="9.140625" style="67"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="71" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" s="71" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>40</v>
       </c>
@@ -7140,8 +7279,14 @@
       <c r="AN1" s="70" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:40" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AO1" s="107" t="s">
+        <v>112</v>
+      </c>
+      <c r="AP1" s="107" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="75" t="s">
         <v>105</v>
       </c>
@@ -7149,7 +7294,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="76">
-        <v>1210</v>
+        <v>210</v>
       </c>
       <c r="D2" s="76">
         <v>7.33</v>
@@ -7191,11 +7336,11 @@
       </c>
       <c r="R2" s="80">
         <f>(Table1[[#This Row],[Reach Length '[meters']]]/(Table1[[#This Row],[Q '[m3/sec']]]/(Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]])))/3600</f>
-        <v>0.37078694452598909</v>
+        <v>6.4351453182196455E-2</v>
       </c>
       <c r="S2" s="80">
         <f>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</f>
-        <v>4.0349473122582369</v>
+        <v>0.70028011204481799</v>
       </c>
       <c r="T2" s="80">
         <v>1</v>
@@ -7208,7 +7353,7 @@
       </c>
       <c r="W2" s="80">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
-        <v>1.21</v>
+        <v>0.21</v>
       </c>
       <c r="X2" s="77">
         <v>1.0510314000000001</v>
@@ -7219,7 +7364,7 @@
       </c>
       <c r="Z2" s="80">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]-Table1[[#This Row],[Start point distance '[meters']]]</f>
-        <v>1210</v>
+        <v>210</v>
       </c>
       <c r="AA2" s="80">
         <f>(Table1[[#This Row],[Tp]]-AN2)*3600</f>
@@ -7227,11 +7372,11 @@
       </c>
       <c r="AB2" s="82">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="AC2" s="82">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>1.21</v>
+        <v>3.5</v>
       </c>
       <c r="AD2" s="82">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
@@ -7239,19 +7384,19 @@
       </c>
       <c r="AE2" s="80">
         <f t="shared" ref="AE2:AE3" si="0">Delta_T__seconds</f>
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="AF2" s="81">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
-        <v>-21.247216671559347</v>
+        <v>-2.8610871909317876</v>
       </c>
       <c r="AG2" s="81">
         <f>(('Reach Propertise'!$F2-'Reach Propertise'!$R2)/'Reach Propertise'!$F2)</f>
-        <v>-3.4512238238414059</v>
+        <v>0.22747355123413618</v>
       </c>
       <c r="AH2" s="81">
         <f>((Table1[[#This Row],[Tt]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Tt]])</f>
-        <v>-1.8400702133905547</v>
+        <v>0.507095252221474</v>
       </c>
       <c r="AI2" s="83">
         <f>Table1[[#This Row],[width '[meters']]]/Table1[[#This Row],[depth '[meters']]]</f>
@@ -7259,7 +7404,7 @@
       </c>
       <c r="AJ2" s="80">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>8086.2197455799997</v>
+        <v>485.17318473479997</v>
       </c>
       <c r="AK2" s="80">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -7275,17 +7420,25 @@
       <c r="AN2" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:40" s="84" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AO2" s="108">
+        <f>FLOOR(C2:C8/Delta_X__meters,1)</f>
+        <v>3</v>
+      </c>
+      <c r="AP2" s="108">
+        <f>((1/1000000)*[1]!Table1[[#This Row],[Cup]]*[1]!Table1[[#This Row],[R ratio]]*[1]!Table1[[#This Row],[Inj Mass]])/[1]!Table1[[#This Row],[Q '[m3/sec']]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="75" t="s">
         <v>106</v>
       </c>
       <c r="B3" s="76">
         <f>C2</f>
-        <v>1210</v>
+        <v>210</v>
       </c>
       <c r="C3" s="76">
-        <v>2175</v>
+        <v>1175</v>
       </c>
       <c r="D3" s="76">
         <v>7.03</v>
@@ -7331,7 +7484,7 @@
       </c>
       <c r="S3" s="80">
         <f>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</f>
-        <v>1.394338026002</v>
+        <v>0.75326307151832184</v>
       </c>
       <c r="T3" s="80">
         <v>1</v>
@@ -7344,7 +7497,7 @@
       </c>
       <c r="W3" s="80">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
-        <v>2.1749999999999998</v>
+        <v>1.175</v>
       </c>
       <c r="X3" s="77">
         <v>0.22527449999999999</v>
@@ -7363,19 +7516,19 @@
       </c>
       <c r="AB3" s="82">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>311</v>
+        <v>44</v>
       </c>
       <c r="AC3" s="82">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>2.1749999999999998</v>
+        <v>19.583333333333332</v>
       </c>
       <c r="AD3" s="82">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>1.21</v>
+        <v>3.5</v>
       </c>
       <c r="AE3" s="80">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="AF3" s="81">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7395,7 +7548,7 @@
       </c>
       <c r="AJ3" s="80">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>6778.20510053</v>
+        <v>406.6923060318</v>
       </c>
       <c r="AK3" s="80">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -7411,17 +7564,25 @@
       <c r="AN3" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:40" s="84" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AO3" s="108">
+        <f>FLOOR(C3:C9/Delta_X__meters,1)</f>
+        <v>19</v>
+      </c>
+      <c r="AP3" s="108">
+        <f>((1/1000000)*[1]!Table1[[#This Row],[Cup]]*[1]!Table1[[#This Row],[R ratio]]*[1]!Table1[[#This Row],[Inj Mass]])/[1]!Table1[[#This Row],[Q '[m3/sec']]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="85" t="s">
         <v>107</v>
       </c>
       <c r="B4" s="76">
         <f t="shared" ref="B4:B8" si="1">C3</f>
-        <v>2175</v>
+        <v>1175</v>
       </c>
       <c r="C4" s="76">
-        <v>3875</v>
+        <v>2875</v>
       </c>
       <c r="D4" s="76">
         <v>7.24</v>
@@ -7467,7 +7628,7 @@
       </c>
       <c r="S4" s="80">
         <f>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</f>
-        <v>0.94978283675010045</v>
+        <v>0.70467758855652618</v>
       </c>
       <c r="T4" s="80">
         <v>1</v>
@@ -7480,7 +7641,7 @@
       </c>
       <c r="W4" s="88">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
-        <v>3.875</v>
+        <v>2.875</v>
       </c>
       <c r="X4" s="86">
         <v>0.11053590000000001</v>
@@ -7499,19 +7660,19 @@
       </c>
       <c r="AB4" s="89">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>815</v>
+        <v>116</v>
       </c>
       <c r="AC4" s="89">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>3.875</v>
+        <v>47.916666666666664</v>
       </c>
       <c r="AD4" s="89">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>2.1749999999999998</v>
+        <v>19.583333333333332</v>
       </c>
       <c r="AE4" s="80">
         <f>Delta_T__seconds</f>
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="AF4" s="81">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7531,7 +7692,7 @@
       </c>
       <c r="AJ4" s="88">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>9500.8611492999989</v>
+        <v>570.05166895799994</v>
       </c>
       <c r="AK4" s="88">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -7543,17 +7704,25 @@
         <v>1.1333</v>
       </c>
       <c r="AN4" s="80"/>
-    </row>
-    <row r="5" spans="1:40" s="84" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AO4" s="108">
+        <f>FLOOR(C4:C10/Delta_X__meters,1)</f>
+        <v>47</v>
+      </c>
+      <c r="AP4" s="108">
+        <f>((1/1000000)*[1]!Table1[[#This Row],[Cup]]*[1]!Table1[[#This Row],[R ratio]]*[1]!Table1[[#This Row],[Inj Mass]])/[1]!Table1[[#This Row],[Q '[m3/sec']]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="85" t="s">
         <v>108</v>
       </c>
       <c r="B5" s="76">
         <f t="shared" si="1"/>
-        <v>3875</v>
+        <v>2875</v>
       </c>
       <c r="C5" s="76">
-        <v>6275</v>
+        <v>5275</v>
       </c>
       <c r="D5" s="76">
         <v>7.51</v>
@@ -7599,7 +7768,7 @@
       </c>
       <c r="S5" s="80">
         <f>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</f>
-        <v>0.70663459502799519</v>
+        <v>0.59402350418688044</v>
       </c>
       <c r="T5" s="80">
         <v>1</v>
@@ -7612,7 +7781,7 @@
       </c>
       <c r="W5" s="88">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
-        <v>6.2750000000000004</v>
+        <v>5.2750000000000004</v>
       </c>
       <c r="X5" s="86">
         <v>5.8002699999999997E-2</v>
@@ -7631,19 +7800,19 @@
       </c>
       <c r="AB5" s="89">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>1776</v>
+        <v>253</v>
       </c>
       <c r="AC5" s="89">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>6.2750000000000004</v>
+        <v>87.916666666666671</v>
       </c>
       <c r="AD5" s="89">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>3.875</v>
+        <v>47.916666666666664</v>
       </c>
       <c r="AE5" s="80">
         <f>Delta_T__seconds</f>
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="AF5" s="81">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7663,7 +7832,7 @@
       </c>
       <c r="AJ5" s="88">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>11085.88435308</v>
+        <v>665.15306118480009</v>
       </c>
       <c r="AK5" s="88">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -7675,17 +7844,25 @@
         <v>2.4666999999999999</v>
       </c>
       <c r="AN5" s="80"/>
-    </row>
-    <row r="6" spans="1:40" s="84" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AO5" s="108">
+        <f>FLOOR(C5:C11/Delta_X__meters,1)</f>
+        <v>87</v>
+      </c>
+      <c r="AP5" s="108">
+        <f>((1/1000000)*[1]!Table1[[#This Row],[Cup]]*[1]!Table1[[#This Row],[R ratio]]*[1]!Table1[[#This Row],[Inj Mass]])/[1]!Table1[[#This Row],[Q '[m3/sec']]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="85" t="s">
         <v>109</v>
       </c>
       <c r="B6" s="76">
         <f t="shared" si="1"/>
-        <v>6275</v>
+        <v>5275</v>
       </c>
       <c r="C6" s="76">
-        <v>8775</v>
+        <v>7775</v>
       </c>
       <c r="D6" s="76">
         <v>9.25</v>
@@ -7731,7 +7908,7 @@
       </c>
       <c r="S6" s="80">
         <f>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</f>
-        <v>0.65290761524656471</v>
+        <v>0.57850218900763994</v>
       </c>
       <c r="T6" s="80">
         <v>1</v>
@@ -7744,7 +7921,7 @@
       </c>
       <c r="W6" s="88">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
-        <v>8.7750000000000004</v>
+        <v>7.7750000000000004</v>
       </c>
       <c r="X6" s="86">
         <v>3.4605400000000001E-2</v>
@@ -7763,19 +7940,19 @@
       </c>
       <c r="AB6" s="89">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>2687</v>
+        <v>383</v>
       </c>
       <c r="AC6" s="89">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>8.7750000000000004</v>
+        <v>129.58333333333334</v>
       </c>
       <c r="AD6" s="89">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>6.2750000000000004</v>
+        <v>87.916666666666671</v>
       </c>
       <c r="AE6" s="80">
         <f>Delta_T__seconds</f>
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="AF6" s="81">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7795,7 +7972,7 @@
       </c>
       <c r="AJ6" s="88">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>18430.574269620003</v>
+        <v>1105.8344561772001</v>
       </c>
       <c r="AK6" s="88">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -7807,17 +7984,25 @@
         <v>3.7332999999999998</v>
       </c>
       <c r="AN6" s="80"/>
-    </row>
-    <row r="7" spans="1:40" s="84" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AO6" s="108">
+        <f>FLOOR(C6:C12/Delta_X__meters,1)</f>
+        <v>129</v>
+      </c>
+      <c r="AP6" s="108">
+        <f>((1/1000000)*[1]!Table1[[#This Row],[Cup]]*[1]!Table1[[#This Row],[R ratio]]*[1]!Table1[[#This Row],[Inj Mass]])/[1]!Table1[[#This Row],[Q '[m3/sec']]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="85" t="s">
         <v>110</v>
       </c>
       <c r="B7" s="76">
         <f t="shared" si="1"/>
-        <v>8775</v>
+        <v>7775</v>
       </c>
       <c r="C7" s="76">
-        <v>11275</v>
+        <v>10275</v>
       </c>
       <c r="D7" s="76">
         <v>9.8000000000000007</v>
@@ -7863,7 +8048,7 @@
       </c>
       <c r="S7" s="80">
         <f>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</f>
-        <v>0.62224473892763099</v>
+        <v>0.56705673547506941</v>
       </c>
       <c r="T7" s="80">
         <v>1</v>
@@ -7876,7 +8061,7 @@
       </c>
       <c r="W7" s="88">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
-        <v>11.275</v>
+        <v>10.275</v>
       </c>
       <c r="X7" s="86">
         <v>2.1080000000000002E-2</v>
@@ -7895,19 +8080,19 @@
       </c>
       <c r="AB7" s="89">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>3623</v>
+        <v>517</v>
       </c>
       <c r="AC7" s="89">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>11.275</v>
+        <v>171.25</v>
       </c>
       <c r="AD7" s="89">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>8.7750000000000004</v>
+        <v>129.58333333333334</v>
       </c>
       <c r="AE7" s="80">
         <f>Delta_T__seconds</f>
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="AF7" s="81">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7927,7 +8112,7 @@
       </c>
       <c r="AJ7" s="88">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>13132.06423686</v>
+        <v>787.92385421159997</v>
       </c>
       <c r="AK7" s="88">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -7939,17 +8124,25 @@
         <v>5.0332999999999997</v>
       </c>
       <c r="AN7" s="80"/>
-    </row>
-    <row r="8" spans="1:40" s="84" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AO7" s="108">
+        <f>FLOOR(C7:C13/Delta_X__meters,1)</f>
+        <v>171</v>
+      </c>
+      <c r="AP7" s="108">
+        <f>((1/1000000)*[1]!Table1[[#This Row],[Cup]]*[1]!Table1[[#This Row],[R ratio]]*[1]!Table1[[#This Row],[Inj Mass]])/[1]!Table1[[#This Row],[Q '[m3/sec']]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="85" t="s">
         <v>111</v>
       </c>
       <c r="B8" s="76">
         <f t="shared" si="1"/>
-        <v>11275</v>
+        <v>10275</v>
       </c>
       <c r="C8" s="76">
-        <v>14775</v>
+        <v>13775</v>
       </c>
       <c r="D8" s="76">
         <v>10</v>
@@ -7995,7 +8188,7 @@
       </c>
       <c r="S8" s="80">
         <f>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</f>
-        <v>0.62784602283447299</v>
+        <v>0.58535221418239358</v>
       </c>
       <c r="T8" s="80">
         <v>1</v>
@@ -8008,7 +8201,7 @@
       </c>
       <c r="W8" s="88">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
-        <v>14.775</v>
+        <v>13.775</v>
       </c>
       <c r="X8" s="86">
         <v>2.0655E-2</v>
@@ -8027,19 +8220,19 @@
       </c>
       <c r="AB8" s="89">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>4706</v>
+        <v>672</v>
       </c>
       <c r="AC8" s="89">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>14.775</v>
+        <v>229.58333333333334</v>
       </c>
       <c r="AD8" s="89">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>11.275</v>
+        <v>171.25</v>
       </c>
       <c r="AE8" s="80">
         <f>Delta_T__seconds</f>
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="AF8" s="81">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8059,7 +8252,7 @@
       </c>
       <c r="AJ8" s="88">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>14727.162258419998</v>
+        <v>883.62973550519985</v>
       </c>
       <c r="AK8" s="88">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8071,18 +8264,57 @@
         <v>6.5369000000000002</v>
       </c>
       <c r="AN8" s="80"/>
-    </row>
-    <row r="9" spans="1:40" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AO8" s="108">
+        <f>FLOOR(C8:C14/Delta_X__meters,1)</f>
+        <v>229</v>
+      </c>
+      <c r="AP8" s="108">
+        <f>((1/1000000)*[1]!Table1[[#This Row],[Cup]]*[1]!Table1[[#This Row],[R ratio]]*[1]!Table1[[#This Row],[Inj Mass]])/[1]!Table1[[#This Row],[Q '[m3/sec']]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" s="90" customFormat="1" x14ac:dyDescent="0.25">
       <c r="X9" s="91"/>
       <c r="Y9" s="92"/>
     </row>
-    <row r="10" spans="1:40" s="90" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" s="90" customFormat="1" x14ac:dyDescent="0.25">
       <c r="X10" s="91"/>
       <c r="Y10" s="92"/>
     </row>
-    <row r="11" spans="1:40" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="X11" s="73"/>
       <c r="Y11" s="74"/>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="Y15" s="98"/>
+      <c r="Z15" s="94"/>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="D16" s="67">
+        <v>18000</v>
+      </c>
+      <c r="Y16" s="99"/>
+      <c r="Z16" s="95"/>
+    </row>
+    <row r="17" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y17" s="100"/>
+      <c r="Z17" s="96"/>
+    </row>
+    <row r="18" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y18" s="101"/>
+      <c r="Z18" s="97"/>
+    </row>
+    <row r="19" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y19" s="100"/>
+      <c r="Z19" s="96"/>
+    </row>
+    <row r="20" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y20" s="101"/>
+      <c r="Z20" s="97"/>
+    </row>
+    <row r="21" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y21" s="103"/>
+      <c r="Z21" s="102"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8160,7 +8392,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8222,7 +8454,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="61">
-        <v>1100</v>
+        <v>100</v>
       </c>
       <c r="B2" s="13">
         <v>1000</v>
@@ -8520,72 +8752,157 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0.15981663310633737</v>
+        <v>0.68015664268852827</v>
       </c>
       <c r="B1">
-        <v>65.097025485873303</v>
+        <v>14.381730614658528</v>
       </c>
       <c r="C1">
-        <v>29.560343977340583</v>
+        <v>53.346954629423969</v>
       </c>
       <c r="D1">
-        <v>30.520218216815454</v>
+        <v>24.944368285190407</v>
       </c>
       <c r="E1">
-        <v>34.073760652701921</v>
+        <v>27.52928439270714</v>
       </c>
       <c r="F1">
-        <v>13.989947841310828</v>
+        <v>15.313694228549927</v>
       </c>
       <c r="G1">
-        <v>34.71653091820702</v>
+        <v>27.453400050271661</v>
       </c>
       <c r="H1">
-        <v>25.841905109265536</v>
+        <v>35.884936034862996</v>
       </c>
       <c r="I1">
-        <v>24.671945258643301</v>
+        <v>21.676550151409781</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.15981663310633737</v>
+        <v>0.31322849740396147</v>
       </c>
       <c r="B2">
-        <v>82.30298751398054</v>
+        <v>36.525382552168367</v>
       </c>
       <c r="C2">
-        <v>29.560343977340583</v>
+        <v>32.534000789767745</v>
       </c>
       <c r="D2">
-        <v>36.083754185453849</v>
+        <v>33.417506117698331</v>
       </c>
       <c r="E2">
-        <v>39.094306447495221</v>
+        <v>38.84840735065351</v>
       </c>
       <c r="F2">
-        <v>17.6876668927755</v>
+        <v>23.277590695310806</v>
       </c>
       <c r="G2">
-        <v>40.197158658042277</v>
+        <v>34.811568463568335</v>
       </c>
       <c r="H2">
-        <v>28.550431143687373</v>
+        <v>32.643688089241856</v>
       </c>
       <c r="I2">
-        <v>26.475009232398943</v>
+        <v>20.812053037658316</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.26698111766955995</v>
+      </c>
+      <c r="B3">
+        <v>33.390806589551822</v>
+      </c>
+      <c r="C3">
+        <v>14.03880466851562</v>
+      </c>
+      <c r="D3">
+        <v>43.206819882737427</v>
+      </c>
+      <c r="E3">
+        <v>45.241875502440102</v>
+      </c>
+      <c r="F3">
+        <v>41.63305266191491</v>
+      </c>
+      <c r="G3">
+        <v>35.359440679528277</v>
+      </c>
+      <c r="H3">
+        <v>31.962756249979922</v>
+      </c>
+      <c r="I3">
+        <v>23.866176447391744</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.35933783316164253</v>
+      </c>
+      <c r="B4">
+        <v>20.372935049446575</v>
+      </c>
+      <c r="C4">
+        <v>18.624112795831529</v>
+      </c>
+      <c r="D4">
+        <v>33.314135015728112</v>
+      </c>
+      <c r="E4">
+        <v>35.177546386489475</v>
+      </c>
+      <c r="F4">
+        <v>28.096184267128709</v>
+      </c>
+      <c r="G4">
+        <v>29.10676961852668</v>
+      </c>
+      <c r="H4">
+        <v>30.806528017469848</v>
+      </c>
+      <c r="I4">
+        <v>23.551261448561682</v>
+      </c>
       <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.34387364708602081</v>
+      </c>
+      <c r="B5">
+        <v>77.369606165605788</v>
+      </c>
+      <c r="C5">
+        <v>62.363966507937029</v>
+      </c>
+      <c r="D5">
+        <v>43.443566400056703</v>
+      </c>
+      <c r="E5">
+        <v>51.712553908003869</v>
+      </c>
+      <c r="F5">
+        <v>26.791796370902254</v>
+      </c>
+      <c r="G5">
+        <v>51.744233499347608</v>
+      </c>
+      <c r="H5">
+        <v>43.34296430768245</v>
+      </c>
+      <c r="I5">
+        <v>33.465758842333642</v>
+      </c>
       <c r="P5" s="39">
         <v>0.68029399999999995</v>
       </c>
@@ -8615,6 +8932,33 @@
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.33506683054146424</v>
+      </c>
+      <c r="B6">
+        <v>60.174042250514447</v>
+      </c>
+      <c r="C6">
+        <v>70.772994369132917</v>
+      </c>
+      <c r="D6">
+        <v>33.197199515206243</v>
+      </c>
+      <c r="E6">
+        <v>41.144595726212735</v>
+      </c>
+      <c r="F6">
+        <v>18.926217222075252</v>
+      </c>
+      <c r="G6">
+        <v>42.521834635580191</v>
+      </c>
+      <c r="H6">
+        <v>37.450196851082339</v>
+      </c>
+      <c r="I6">
+        <v>27.08994181247148</v>
+      </c>
       <c r="P6" s="39">
         <v>0.31323899999999999</v>
       </c>
@@ -8644,6 +8988,33 @@
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.45280611092443795</v>
+      </c>
+      <c r="B7">
+        <v>27.460498428617271</v>
+      </c>
+      <c r="C7">
+        <v>35.458238134848095</v>
+      </c>
+      <c r="D7">
+        <v>35.26734159215561</v>
+      </c>
+      <c r="E7">
+        <v>39.998500617030622</v>
+      </c>
+      <c r="F7">
+        <v>25.0441175460994</v>
+      </c>
+      <c r="G7">
+        <v>35.320773438636586</v>
+      </c>
+      <c r="H7">
+        <v>37.394201405106315</v>
+      </c>
+      <c r="I7">
+        <v>28.194582095621172</v>
+      </c>
       <c r="P7" s="39">
         <v>0.26703500000000002</v>
       </c>
@@ -9434,15 +9805,15 @@
     </row>
     <row r="28" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F28" s="45"/>
-      <c r="G28" s="94" t="s">
+      <c r="G28" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="H28" s="95"/>
-      <c r="I28" s="95"/>
-      <c r="J28" s="95"/>
-      <c r="K28" s="95"/>
-      <c r="L28" s="95"/>
-      <c r="M28" s="96"/>
+      <c r="H28" s="105"/>
+      <c r="I28" s="105"/>
+      <c r="J28" s="105"/>
+      <c r="K28" s="105"/>
+      <c r="L28" s="105"/>
+      <c r="M28" s="106"/>
     </row>
     <row r="29" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F29" s="46" t="s">

</xml_diff>